<commit_message>
all relic and translate
</commit_message>
<xml_diff>
--- a/全部元驱动效果（暂定）v3.0.xlsx
+++ b/全部元驱动效果（暂定）v3.0.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepository\DSP_Battle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD55713-A1E5-4CC0-9EF6-382E19305EF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121AC532-C223-4318-A45D-4B6143EBFE81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="传说" sheetId="1" r:id="rId1"/>
-    <sheet name="史诗" sheetId="2" r:id="rId2"/>
-    <sheet name="稀有" sheetId="3" r:id="rId3"/>
-    <sheet name="普通" sheetId="4" r:id="rId4"/>
-    <sheet name="底层" sheetId="5" r:id="rId5"/>
+    <sheet name="传说0" sheetId="1" r:id="rId1"/>
+    <sheet name="史诗1" sheetId="2" r:id="rId2"/>
+    <sheet name="稀有2" sheetId="3" r:id="rId3"/>
+    <sheet name="普通3" sheetId="4" r:id="rId4"/>
+    <sheet name="公理4" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="169">
   <si>
     <t>功能</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -44,10 +44,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>制造厂在制造原材料至少2种的配方时，每产出1个产物，会返还1个第1位置的原材料</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>战斗</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -108,10 +104,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>不朽之守护</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>凯旋</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -192,10 +184,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>引力碎裂</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>恒星炮充能速度+50%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -228,10 +216,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>光刻机</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>矩阵雨</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -256,10 +240,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>拥有巨构的星系，行星的最大护盾上限提升，根据巨构的能量产出，最多提升50%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>聚能环 II</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -292,24 +272,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>所有导弹对首要目标造成100%</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>额外伤害</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>撕裂力场</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -323,10 +285,6 @@
   </si>
   <si>
     <t>吞噬者</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>五叶草</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -364,24 +322,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>你对敌舰造成的任何伤害有10%的概率造成100%独立的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>额外伤害</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>巨构的太阳帆吸附速度提升100%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -390,10 +330,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>来自行星护盾生成器的护盾充能速度提升50%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>强度*10 敌舰击杀经验</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -410,10 +346,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>生产芯片、量子芯片时，来自增产剂的增产效果加强50%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>伊卡洛斯的研究速度+400%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -430,10 +362,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>永恒之盘</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>巨构在计算能量水平时，恒星光度显著增加（大约相当于所有恒星光度+1.0）</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -442,10 +370,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>每过一秒，如果伊卡洛斯移动过，就有12%的概率获得一个多功能集成组件（考虑在2.2.5削弱</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>编织者</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -498,22 +422,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>每当击杀敌军单位时，无消耗地略微推进当前科技的研究进度（黑雾矩阵科技除外，研究速度科技可以略微加成推进量）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑雾矩阵掉落减半，放弃解译圣物无法获得黑雾矩阵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>死亡时，你降低一级功勋阶级并清空当前等级的功勋点数</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>所有防御设施的弹药组每次被消耗时，立刻回填一组相同的弹药。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>战斗无人机各项能量消耗-40%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -526,37 +438,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>使用导弹和动能子弹，在射击时有5%概率回填一组弹药</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>击杀黑雾单位时，获得沙土</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>黑雾获得经验+100%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>能量武器造成相当于20%的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>额外伤害</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>建筑被毁时，立刻少量推进随机星系的巨构的建造进度</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -582,10 +464,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>快速晋升</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>功勋点数获取+25%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -594,37 +472,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>敌军掉落黑雾专属物品时，额外掉落等量所有类型的黑雾专属物品（无法越级掉落）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>卢登的封印</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>虚空冲击</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>防御塔的爆发持续时间+200%</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>引力导弹对首要目标造成1000%</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>额外伤害</t>
-    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -684,19 +532,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>你的所有概率判定均会更加幸运（元驱动的概率判定进行两次判定，有一次通过即算成功；获取元驱动时，刷新更高稀有度的概率也略微增加）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>所有具有概率的元驱动，判定成功几率减半</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>获取此元驱动时，将左侧栏位最顶端的三个元驱动永久保存在符文之书中，保留他们的效果但是其不再占用圣物栏位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>解译元驱动的所需时间+30min</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -733,31 +573,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>击杀黑雾单位时，有0.1%几率掉落额外的宇宙矩阵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次击毁太空黑雾单位，有4%概率在背包直接获取1个反物质燃料棒或翘曲器，无视科技解锁进度</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>底层：每拥有一个底层元驱动，黑雾获得经验+20%，威胁度增长速度+5%。底层元驱动无法被移除。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>每解锁或升级一个科技，少量推进随机巨构的建造进度</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次击杀黑雾单位，有概率略微推进随机星系的巨构的建造进度。地面黑雾单位提供的点数较少</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>伊卡洛斯的能量盾被打破时，根据机甲燃烧室储备立刻回复最多100%的能量盾，并消耗相当于回复量2倍的燃烧室储备。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>地面和太空舰队中的单位将要承受伤害时，如果伊卡洛斯的能量盾充能高于50%，则免疫该次伤害，转而由伊卡洛斯的能量盾承担，且伤害降低50%。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -833,14 +649,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>所有防御设施在装填一组弹药时，有35%概率回填两组弹药。备选方案：导弹和子弹在命中时，有15%概率从原地额外发射一发弹药攻击随机的敌军单位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>大幅强化干扰塔的效果</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>行星护盾和伊卡洛斯的能量盾获得10%伤害减免，且它们会将所有被减免或被规避的伤害全额回敬给攻击者作为</t>
     </r>
@@ -870,27 +678,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>行星护盾和伊卡洛斯的护盾获得20%伤害减免，如果单次伤害超过当前护盾量的5%，则转而减免80%。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>伊卡洛斯被摧毁时，立刻回复全部的生命值和能量盾，并获得30s的伤害免疫，这个效果每20min只能触发一次</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>你的伤害将永久无视黑雾单位的护甲。不占用元驱动槽位</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>下次伊卡洛斯被毁时，可以免费原地重组，不占用元驱动槽位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>基于已解锁的科技，立刻获得大量普通矩阵（异星矩阵和宇宙矩阵除外），不占用元驱动槽位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>每过一秒，如果伊卡洛斯移动过，就有5%的概率获得一个多功能集成组件</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -911,12 +703,218 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Luden's Tempest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有防御设施的弹药组每次被消耗时，立刻回填一组完全相同的弹药。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有防御设施在装填一组弹药时，有35%概率回填两组完全相同的弹药（弹药储备不会超过100组）。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行星护盾和伊卡洛斯的护盾获得20%伤害减免，如果单次伤害超过当前护盾量的1%，则转而减免80%。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>伊卡洛斯的能量盾被打破时，根据机甲燃烧室当前储备立刻回复最多100%的能量盾，这需要消耗相当于回复量2倍的燃烧室能量。一分钟内反复触发此效果会使消耗倍率逐渐增加至最高20倍。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地面和太空舰队中的单位将要承受伤害时，如果伊卡洛斯的能量盾充能高于50%，则免疫该次伤害，转而由伊卡洛斯的能量盾承担一半的伤害。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>行星护盾获得50%额外的充能量</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有防御设施在装填时有40%概率回填一组弹药</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级咯</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>我超！铲！Spatula</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>It must do something…</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>大幅强化干扰胶囊和压制胶囊的效果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御塔的超新星持续时间+200%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>能量循环</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每过一秒，如果伊卡洛斯移动过，就有3%的概率获得一个多功能集成组件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每过一秒，如果伊卡洛斯移动过，就有8%的概率获得一个多功能集成组件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>动能武器伤害、爆破武器伤害、能量武器伤害+10%，不占用元驱动槽位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆破武器伤害+40%，不占用元驱动槽位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得基于当前阶级的少量功勋点数，不占用元驱动槽位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>能量武器伤害+10%，不占用元驱动槽位</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御塔的超新星冷却和蓄能时间-50%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>你对敌舰造成的任何伤害有10%的概率造成100%的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>额外伤害</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的所有概率判定均会更加幸运（元驱动的概率判定进行两次判定，有一次通过即算成功；获取元驱动时，刷新更高稀有度的概率也略微增加。以及其他隐藏效果，比如行窃预兆会偷到黄棒而非黑棒）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次击毁太空黑雾单位，有3%概率在背包直接获取1个反物质燃料棒或翘曲器，无视科技解锁进度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不朽之守护（Aegis of the immortal）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>伊卡洛斯即将被摧毁时，转而立刻回复全部的生命值和能量盾，并获得30s的伤害免疫，这个效果每20min只能触发一次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>伊卡洛斯被毁时，可以选择消耗复活币来无消耗地重新部署或原地重组。复活币最多叠加10个，且不占用元驱动槽位。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ui?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5201黑雾矩阵</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5203物质重组器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5202硅基神经元</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5204负熵奇点</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5205核心素</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>地面黑雾单位掉落黑雾矩阵时，有30%几率掉落双倍的黑雾矩阵</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑雾单位掉落的沙土加倍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑被毁时，微量推进随机星系的巨构的建造进度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>解译元驱动的所需时间+15min</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>公理级：每拥有一个公理级元驱动，黑雾获得经验+50%，并获得5%伤害减免。公理级元驱动无法被移除。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑雾单位掉落黑雾专属物品时，额外掉落一半数量的所有其他类型的黑雾专属物品（无法越级掉落）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每当击杀敌军单位时，无消耗地略微推进当前科技的研究进度（黑雾矩阵科技除外，研究速度科技可以加成推进量）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑雾矩阵掉落减半，放弃解译元驱动的解码轨时不会获得黑雾矩阵</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>永恒之环</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>星辰封印</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>每击杀一定数量的黑雾单位，略微推进随机星系的巨构的建造进度。地面黑雾单位提供的点数较少</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>制造厂和星际组装厂在制造原材料至少2种的配方时，每产出1个产物，会返还1个第1位置的原材料</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外UI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外ui</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,6 +971,29 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFF73131"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1024,7 +1045,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1126,6 +1147,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1145,22 +1203,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1198,9 +1251,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - 着色 5" xfId="5" builtinId="47"/>
@@ -1229,6 +1312,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219808</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>109903</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>192660</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>160846</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558E7374-27F9-4244-9394-88F169953B59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10770577" y="2483826"/>
+          <a:ext cx="6171429" cy="2761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1494,289 +1626,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.375" customWidth="1"/>
-    <col min="4" max="4" width="80" customWidth="1"/>
-    <col min="5" max="5" width="18.75" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="3.75" customWidth="1"/>
+    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="5" max="5" width="80" customWidth="1"/>
+    <col min="6" max="6" width="18.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>0</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="11" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>0</v>
+      </c>
+      <c r="B10" s="15">
+        <v>8</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>0</v>
+      </c>
+      <c r="B11" s="11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>0</v>
+      </c>
+      <c r="B12" s="11">
+        <v>10</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>0</v>
+      </c>
+      <c r="B19">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
         <v>0</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
+      <c r="B20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
-        <v>2</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="B21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>0</v>
+      </c>
+      <c r="B26">
         <v>24</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
-        <v>3</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="16">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
-        <v>4</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="B27">
         <v>25</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="16">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>5</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>6</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
-        <v>7</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
-        <v>8</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
-        <v>9</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
-        <v>10</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="B28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
+        <v>0</v>
+      </c>
+      <c r="B29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
+        <v>0</v>
+      </c>
+      <c r="B30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
+        <v>0</v>
+      </c>
+      <c r="B31">
         <v>29</v>
       </c>
     </row>
@@ -1784,324 +2011,439 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32C589E-18DE-4F43-A43B-F15B47046B0D}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="107.375" customWidth="1"/>
+    <col min="1" max="1" width="4" style="11" customWidth="1"/>
+    <col min="2" max="2" width="3.625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="24.125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="16" style="11" customWidth="1"/>
+    <col min="5" max="5" width="107.375" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>1</v>
+      </c>
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>1</v>
+      </c>
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11">
+        <v>6</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11">
+        <v>7</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11">
+        <v>8</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D10" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="11">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="G10" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11">
+        <v>10</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11">
+        <v>11</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11">
+        <v>13</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>1</v>
+      </c>
+      <c r="B16" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>1</v>
+      </c>
+      <c r="B17" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>1</v>
+      </c>
+      <c r="B18" s="11">
+        <v>16</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>1</v>
+      </c>
+      <c r="B19" s="11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>1</v>
+      </c>
+      <c r="B20" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>1</v>
+      </c>
+      <c r="B22" s="11">
         <v>20</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B23" s="11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3">
+      <c r="B24" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="B25" s="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>1</v>
+      </c>
+      <c r="B26" s="11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
+        <v>1</v>
+      </c>
+      <c r="B27" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>1</v>
+      </c>
+      <c r="B28" s="11">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E5">
+      <c r="B29" s="11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6">
+      <c r="B30" s="11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="B31" s="11">
         <v>29</v>
       </c>
     </row>
@@ -2114,355 +2456,509 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710ABCAC-BF77-4375-AD1C-5040C284D7FE}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-    <col min="4" max="4" width="116" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="3.5" customWidth="1"/>
+    <col min="3" max="3" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="99.5" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="E8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="23"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>2</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="B31">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" t="s">
-        <v>79</v>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2473,393 +2969,538 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36FF14D-DAA7-4EFE-B46C-89F65B92B81C}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
-    <col min="4" max="4" width="94.875" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="3.375" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="97.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
         <v>18</v>
       </c>
-      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
         <v>19</v>
       </c>
-      <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
         <v>20</v>
       </c>
-      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
         <v>21</v>
       </c>
-      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
         <v>22</v>
       </c>
-      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
         <v>23</v>
       </c>
-      <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
         <v>24</v>
       </c>
-      <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
         <v>25</v>
       </c>
-      <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
         <v>26</v>
       </c>
-      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
         <v>27</v>
       </c>
-      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
         <v>28</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="11" t="s">
+      <c r="C30" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" s="11" t="s">
+      <c r="D31" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2871,172 +3512,257 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F59722-8E1B-469E-AA07-25FE093F2633}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="26"/>
-    <col min="2" max="2" width="11.375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="9" style="26"/>
-    <col min="4" max="4" width="56.875" style="26" customWidth="1"/>
-    <col min="5" max="6" width="50.25" style="26" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="5.25" style="21" customWidth="1"/>
+    <col min="2" max="2" width="3.625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="9" style="21"/>
+    <col min="5" max="5" width="56.875" style="21" customWidth="1"/>
+    <col min="6" max="6" width="50.25" style="21" customWidth="1"/>
+    <col min="7" max="7" width="9.75" style="21" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="23" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="F2" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21">
+        <v>4</v>
+      </c>
+      <c r="B3" s="19">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <v>4</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24">
-        <v>0</v>
-      </c>
-      <c r="B3" s="24" t="s">
+      <c r="G5" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21">
+        <v>4</v>
+      </c>
+      <c r="B6" s="19">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="D6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21">
+        <v>4</v>
+      </c>
+      <c r="B7" s="19">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24">
+      <c r="E7" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="21">
         <v>1</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24">
-        <v>2</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="H7" s="21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="21">
         <v>4</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24">
+      <c r="B8" s="19">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="E8" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="21">
         <v>4</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="26">
+      <c r="B9" s="19">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24">
-        <v>4</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="24">
-        <v>5</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="24">
-        <v>6</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>130</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="21">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3048,7 +3774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B99AA0-1784-4B08-9400-9B1D1E5D5BBD}">
   <dimension ref="A1:C900"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A397" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>